<commit_message>
Updated ITA_grids model - 2025-08-15 10:43
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59499B42-9075-4123-ADB6-AA0792E262A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48E000AA-5135-4290-A57A-6BC79C664320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7647,7 +7647,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AF76D70-D4EC-FC4C-FA90-A72355B25740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74E34D96-2F66-F7F7-D934-6351D9EA7DDF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7702,7 +7702,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3667CEE0-6D09-63F9-899A-1E252949BA60}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CF26D00-1C2F-4444-0169-B7CD6BC1DC68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7757,7 +7757,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68FAA4D0-8BB5-C24A-CB4B-195C6A70E0CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EFB9843-DCE9-D04F-E458-30697624C88D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7812,7 +7812,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1C22333-FC19-F2BA-B802-1063412D92AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A0006FD-6D83-FC7B-6CC5-D6170B1A7A90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10315,7 +10315,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF0A175-6936-4790-9054-B172BDF3A5A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FFCDE4-4AF7-4611-9C42-031DD5CE637F}">
   <dimension ref="A1:AG319"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22465,7 +22465,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B27EAA-F1C7-4AC8-90FD-3A2BD9578971}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DD5CB1-7DBD-48F0-A70E-396BA67702EF}">
   <dimension ref="A1:O322"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34677,7 +34677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFA3E5FA-D61F-4C4B-BBB8-F5F30691E967}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E840838-9A2D-4860-97C8-1CF39F79E2C3}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA_grids model - 2025-08-15 15:43
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48E000AA-5135-4290-A57A-6BC79C664320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3531C8FC-E80F-45D1-9205-D6540EA534C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7647,7 +7647,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74E34D96-2F66-F7F7-D934-6351D9EA7DDF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FBE3634-999D-1A84-7938-81480022FEA3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7702,7 +7702,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CF26D00-1C2F-4444-0169-B7CD6BC1DC68}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A40A7C3F-F41D-1E94-6494-51A4BE452D86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7757,7 +7757,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EFB9843-DCE9-D04F-E458-30697624C88D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7A0EFF3-FE64-BF1B-F064-56DC2B28D8AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7812,7 +7812,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A0006FD-6D83-FC7B-6CC5-D6170B1A7A90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA99B593-938F-84AF-4B78-F168B98C5749}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10315,7 +10315,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FFCDE4-4AF7-4611-9C42-031DD5CE637F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D85ABB6-54FF-4230-BE91-1764CE65A852}">
   <dimension ref="A1:AG319"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22465,7 +22465,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DD5CB1-7DBD-48F0-A70E-396BA67702EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8282C4-0348-4C07-8326-B686FB3081E8}">
   <dimension ref="A1:O322"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34677,7 +34677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E840838-9A2D-4860-97C8-1CF39F79E2C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAA256E-D4F8-4677-BDD1-78BEF4E1B1B1}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>